<commit_message>
added specifications for plexiglass plate
</commit_message>
<xml_diff>
--- a/bom.xlsx
+++ b/bom.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\tungsten-nas.fmi.ch\tungsten\scratch\gluthi\zellmart\code\el_commutador\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D35CF9F6-5CFE-41D2-B129-C5EA227ECD27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D4FC97A-CBCA-46DD-A7BC-86FA48863322}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-7536" yWindow="-15420" windowWidth="23040" windowHeight="12204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16032" yWindow="-15324" windowWidth="23040" windowHeight="12204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="52">
   <si>
     <t>Description</t>
   </si>
@@ -172,6 +172,15 @@
   </si>
   <si>
     <t>from this repository, send to PCB fab (e.g. Aisler in Europe)</t>
+  </si>
+  <si>
+    <t>Plexiglass plate, 5mm thick, with cutouts</t>
+  </si>
+  <si>
+    <t>this repository, ideally commission at your instituions workshop</t>
+  </si>
+  <si>
+    <t>1</t>
   </si>
 </sst>
 </file>
@@ -502,7 +511,7 @@
   <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -825,10 +834,16 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
+      <c r="A25" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
+      <c r="D25" s="2" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="2"/>

</xml_diff>